<commit_message>
add genbank result of datarank v2
</commit_message>
<xml_diff>
--- a/data/experiments/results.xlsx
+++ b/data/experiments/results.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3030" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="datarank" sheetId="1" r:id="rId1"/>
+    <sheet name="datarank_v2" sheetId="2" r:id="rId2"/>
+    <sheet name="pagerank" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>algorithm:datarank</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -69,6 +71,22 @@
   </si>
   <si>
     <t>revised version(check)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>algorithm:datarank_v2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>beta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>forward:1-alpha</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>backward:beta</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -478,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -500,17 +518,6 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
@@ -528,24 +535,6 @@
       <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="7">
@@ -563,20 +552,6 @@
       <c r="E3" s="6">
         <v>-8.6920912663615503E-4</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.149879678413879</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0.149894040581977</v>
-      </c>
-      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
@@ -594,20 +569,6 @@
       <c r="E4" s="8">
         <v>-8.2981553194450604E-3</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.149879678413879</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="8">
-        <v>-5.0933375709802699E-2</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
@@ -625,18 +586,6 @@
       <c r="E5" s="8">
         <v>4.4279167308540701E-2</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0.149879678413879</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
@@ -654,18 +603,6 @@
       <c r="E6" s="8">
         <v>3.4809877951280703E-2</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0.15755028460432899</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
@@ -683,22 +620,6 @@
       <c r="E7" s="8">
         <v>9.1606957031747496E-2</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0.15755028460432899</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0.15755588103264501</v>
-      </c>
-      <c r="L7" s="8">
-        <v>-5.0451163380993203E-2</v>
-      </c>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
@@ -716,18 +637,6 @@
       <c r="E8" s="8">
         <v>7.2824815996142794E-2</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0.15755028460432899</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
@@ -745,18 +654,6 @@
       <c r="E9" s="8">
         <v>-2.92411016889653E-2</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0.159741542580674</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
@@ -774,20 +671,6 @@
       <c r="E10" s="8">
         <v>-2.8432566576654099E-2</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="J10" s="8">
-        <v>0.15974335604540901</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="8">
-        <v>-5.0288965677241497E-2</v>
-      </c>
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
@@ -805,18 +688,6 @@
       <c r="E11" s="8">
         <v>8.7845794012065496E-3</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0.15974335604540901</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
@@ -999,4 +870,901 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.75" customWidth="1"/>
+    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="4" max="4" width="14.75" customWidth="1"/>
+    <col min="5" max="5" width="22.25" customWidth="1"/>
+    <col min="6" max="6" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.16732515469086501</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.167786226660851</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.10612083534611499</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.105550667756504</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>-0.138366130536939</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="7">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>-0.138366130536939</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-0.16680670635632</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>-0.16680670635632</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>-0.20064574260235299</v>
+      </c>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
+        <v>20</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>-0.20064600597264301</v>
+      </c>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7">
+        <v>20</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>-0.22937851504088699</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7">
+        <v>20</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>-0.22937848981526701</v>
+      </c>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.15834969330333901</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.15824305717044701</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.12893431014342599</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A18" s="7">
+        <v>5</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0.12867122132689901</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A19" s="7">
+        <v>5</v>
+      </c>
+      <c r="B19" s="7">
+        <v>5</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5.3416589194425601E-2</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="7">
+        <v>5</v>
+      </c>
+      <c r="B20" s="7">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="8">
+        <v>5.3416589194425802E-2</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A21" s="7">
+        <v>5</v>
+      </c>
+      <c r="B21" s="7">
+        <v>5</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="8">
+        <v>-7.0282122882539599E-2</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A22" s="7">
+        <v>5</v>
+      </c>
+      <c r="B22" s="7">
+        <v>5</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="8">
+        <v>-7.0282122882539599E-2</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A23" s="7">
+        <v>5</v>
+      </c>
+      <c r="B23" s="7">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="8">
+        <v>2.2160466980396198E-2</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A24" s="7">
+        <v>5</v>
+      </c>
+      <c r="B24" s="7">
+        <v>20</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="8">
+        <v>2.21598482080612E-2</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A25" s="7">
+        <v>5</v>
+      </c>
+      <c r="B25" s="7">
+        <v>20</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="8">
+        <v>-0.12035305807387001</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A26" s="7">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7">
+        <v>20</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="8">
+        <v>-0.120353249554302</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A27" s="7">
+        <v>20</v>
+      </c>
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0.15313922148498199</v>
+      </c>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A28" s="7">
+        <v>20</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.15313922148498199</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A29" s="7">
+        <v>20</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.13266509586470199</v>
+      </c>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A30" s="7">
+        <v>20</v>
+      </c>
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0.13266509586470199</v>
+      </c>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A31" s="7">
+        <v>20</v>
+      </c>
+      <c r="B31" s="7">
+        <v>5</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0.108027884460389</v>
+      </c>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A32" s="7">
+        <v>20</v>
+      </c>
+      <c r="B32" s="7">
+        <v>5</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0.108027884460389</v>
+      </c>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A33" s="7">
+        <v>20</v>
+      </c>
+      <c r="B33" s="7">
+        <v>5</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E33" s="8">
+        <v>2.3965435250042199E-2</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A34" s="7">
+        <v>20</v>
+      </c>
+      <c r="B34" s="7">
+        <v>5</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E34" s="8">
+        <v>2.3965435250042199E-2</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A35" s="7">
+        <v>20</v>
+      </c>
+      <c r="B35" s="7">
+        <v>20</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="8">
+        <v>9.1612494841683406E-2</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A36" s="7">
+        <v>20</v>
+      </c>
+      <c r="B36" s="7">
+        <v>20</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E36" s="8">
+        <v>9.1614115691380504E-2</v>
+      </c>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A37" s="7">
+        <v>20</v>
+      </c>
+      <c r="B37" s="7">
+        <v>20</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E37" s="8">
+        <v>-9.2409072476452997E-3</v>
+      </c>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A38" s="7">
+        <v>20</v>
+      </c>
+      <c r="B38" s="7">
+        <v>20</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="8">
+        <v>-9.2410588069189708E-3</v>
+      </c>
+      <c r="F38" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="26.375" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="22.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.149879678413879</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.149894040581977</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.149879678413879</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="8">
+        <v>-5.0933375709802699E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.149879678413879</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.15755028460432899</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.15755028460432899</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.15755588103264501</v>
+      </c>
+      <c r="F7" s="8">
+        <v>-5.0451163380993203E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.15755028460432899</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.159741542580674</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.15974335604540901</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8">
+        <v>-5.0288965677241497E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.15974335604540901</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
descrption of datarank v2
</commit_message>
<xml_diff>
--- a/data/experiments/results.xlsx
+++ b/data/experiments/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="8610" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="datarank" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="pagerank" sheetId="3" r:id="rId3"/>
     <sheet name="comparing" sheetId="7" r:id="rId4"/>
     <sheet name="decay_time" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>algorithm:datarank</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -132,6 +133,14 @@
   </si>
   <si>
     <t>delta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">absolute diff of decay time </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg absolute value of corr</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -267,6 +276,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -474,11 +484,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276206768"/>
-        <c:axId val="276207328"/>
+        <c:axId val="272477152"/>
+        <c:axId val="272477712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276206768"/>
+        <c:axId val="272477152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,6 +534,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -590,12 +601,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276207328"/>
+        <c:crossAx val="272477712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276207328"/>
+        <c:axId val="272477712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,6 +657,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -712,9 +724,318 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276206768"/>
+        <c:crossAx val="272477152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>avg _figshare</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avg absolute value of corr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$24:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.8750105E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4190679000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8795827000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8979356000000006E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="484191760"/>
+        <c:axId val="484192880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="484191760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="484192880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="484192880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="484191760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -984,8 +1305,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276210128"/>
-        <c:axId val="276210688"/>
+        <c:axId val="275602224"/>
+        <c:axId val="275602784"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1176,7 +1497,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276210128"/>
+        <c:axId val="275602224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,12 +1643,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276210688"/>
+        <c:crossAx val="275602784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276210688"/>
+        <c:axId val="275602784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1445,7 +1766,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276210128"/>
+        <c:crossAx val="275602224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1534,6 +1855,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1596,7 +1918,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>decay_time!$F$1:$F$4</c:f>
+              <c:f>decay_time!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1617,7 +1939,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>decay_time!$G$1:$G$4</c:f>
+              <c:f>decay_time!$G$2:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1646,11 +1968,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276213488"/>
-        <c:axId val="276214048"/>
+        <c:axId val="275605584"/>
+        <c:axId val="275606144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276213488"/>
+        <c:axId val="275605584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,6 +2023,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1767,12 +2090,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276214048"/>
+        <c:crossAx val="275606144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276214048"/>
+        <c:axId val="275606144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,6 +2149,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1892,7 +2216,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276213488"/>
+        <c:crossAx val="275605584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2045,7 +2369,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>decay_time!$F$16:$F$19</c:f>
+              <c:f>decay_time!$F$24:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2053,10 +2377,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>19</c:v>
@@ -2066,7 +2390,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>decay_time!$G$16:$G$19</c:f>
+              <c:f>decay_time!$G$24:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2074,10 +2398,10 @@
                   <c:v>1.8750105E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3.4190679000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1.8795827000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.4190679000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6.8979356000000006E-2</c:v>
@@ -2095,11 +2419,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276216288"/>
-        <c:axId val="276216848"/>
+        <c:axId val="276126384"/>
+        <c:axId val="276126944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276216288"/>
+        <c:axId val="276126384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2217,12 +2541,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276216848"/>
+        <c:crossAx val="276126944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276216848"/>
+        <c:axId val="276126944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2340,7 +2664,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276216288"/>
+        <c:crossAx val="276126384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2612,11 +2936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276219088"/>
-        <c:axId val="276219648"/>
+        <c:axId val="276129184"/>
+        <c:axId val="276129744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276219088"/>
+        <c:axId val="276129184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2734,12 +3058,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276219648"/>
+        <c:crossAx val="276129744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276219648"/>
+        <c:axId val="276129744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,7 +3177,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276219088"/>
+        <c:crossAx val="276129184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3125,8 +3449,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276222448"/>
-        <c:axId val="277004240"/>
+        <c:axId val="276132544"/>
+        <c:axId val="276133104"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3317,7 +3641,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276222448"/>
+        <c:axId val="276132544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,12 +3759,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277004240"/>
+        <c:crossAx val="276133104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277004240"/>
+        <c:axId val="276133104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3553,7 +3877,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276222448"/>
+        <c:crossAx val="276132544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3602,7 +3926,1058 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>avg_gene</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>decay_time!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avg absolute value of corr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>decay_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.8819157000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.117386477</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.103998375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18237620500000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="349008352"/>
+        <c:axId val="349010592"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>decay_time!$F$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>absolute diff of decay time </c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>decay_time!$F$2:$F$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>19</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="349008352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="349010592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="349010592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="349008352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>avg_figshare</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>decay_time!$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avg absolute value of corr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>decay_time!$G$24:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.8750105E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4190679000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8795827000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8979356000000006E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="470480272"/>
+        <c:axId val="349586880"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>decay_time!$F$23</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>absolute diff of decay time </c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>decay_time!$F$24:$F$27</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>19</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="470480272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="349586880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="349586880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470480272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>avg_gene</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avg absolute value of corr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.8819157000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.117386477</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.103998375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18237620500000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="473666864"/>
+        <c:axId val="473663504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="473666864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473663504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="473663504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473666864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3808,6 +5183,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4324,8 +5819,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4352,8 +5847,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4454,7 +5949,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4486,10 +5981,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4529,23 +6024,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4650,8 +6144,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4783,20 +6277,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4810,17 +6303,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4840,7 +6322,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5356,7 +6838,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5872,7 +7354,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6388,7 +7870,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6885,6 +8367,2031 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -7086,6 +10593,131 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="图表 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="图表 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8608,7 +12240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -9370,8 +13002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="R57" sqref="R57"/>
+    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9389,11 +13021,11 @@
       <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>7.8819157000000001E-2</v>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -9407,10 +13039,10 @@
         <v>8.6920900000000002E-4</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.117386477</v>
+        <v>7.8819157000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -9424,10 +13056,10 @@
         <v>8.2981549999999998E-3</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>0.103998375</v>
+        <v>0.117386477</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -9441,10 +13073,10 @@
         <v>8.7845790000000007E-3</v>
       </c>
       <c r="F4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G4">
-        <v>0.18237620500000001</v>
+        <v>0.103998375</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -9457,6 +13089,12 @@
       <c r="C5">
         <v>1.0656568E-2</v>
       </c>
+      <c r="F5">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>0.18237620500000001</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
@@ -9602,12 +13240,6 @@
       <c r="C16">
         <v>9.1606957000000003E-2</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>1.8750105E-2</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
@@ -9619,12 +13251,6 @@
       <c r="C17">
         <v>7.2824816000000001E-2</v>
       </c>
-      <c r="F17">
-        <v>15</v>
-      </c>
-      <c r="G17">
-        <v>1.8795827000000001E-2</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
@@ -9636,12 +13262,6 @@
       <c r="C18">
         <v>5.8875332000000002E-2</v>
       </c>
-      <c r="F18">
-        <v>4</v>
-      </c>
-      <c r="G18">
-        <v>3.4190679000000002E-2</v>
-      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
@@ -9661,10 +13281,44 @@
         <f>AVERAGE(C16:C19)</f>
         <v>6.8979355749999999E-2</v>
       </c>
-      <c r="F19">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1.8750105E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>3.4190679000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F26">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>1.8795827000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F27">
         <v>19</v>
       </c>
-      <c r="G19">
+      <c r="G27">
         <v>6.8979356000000006E-2</v>
       </c>
     </row>
@@ -9878,9 +13532,107 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="G16:G28">
-    <sortCondition ref="G16"/>
+  <sortState ref="F24:G27">
+    <sortCondition ref="F23"/>
   </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>7.8819157000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.117386477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0.103998375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>0.18237620500000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>1.8750105E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>3.4190679000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>1.8795827000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>6.8979356000000006E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
some update for figshare pagerank results
</commit_message>
<xml_diff>
--- a/data/experiments/results.xlsx
+++ b/data/experiments/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8610" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="4"/>
+    <workbookView xWindow="9540" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="datarank" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>algorithm:datarank</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -70,10 +70,6 @@
   </si>
   <si>
     <t>genbank's correlation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>revised version(check)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -276,7 +272,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -484,11 +479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="272477152"/>
-        <c:axId val="272477712"/>
+        <c:axId val="250175264"/>
+        <c:axId val="250175824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="272477152"/>
+        <c:axId val="250175264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +529,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -601,12 +595,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272477712"/>
+        <c:crossAx val="250175824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="272477712"/>
+        <c:axId val="250175824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +651,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -724,7 +717,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="272477152"/>
+        <c:crossAx val="250175264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -927,11 +920,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="484191760"/>
-        <c:axId val="484192880"/>
+        <c:axId val="335757184"/>
+        <c:axId val="335757744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="484191760"/>
+        <c:axId val="335757184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +967,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484192880"/>
+        <c:crossAx val="335757744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -982,7 +975,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="484192880"/>
+        <c:axId val="335757744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,7 +1026,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484191760"/>
+        <c:crossAx val="335757184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1305,8 +1298,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="275602224"/>
-        <c:axId val="275602784"/>
+        <c:axId val="251542992"/>
+        <c:axId val="251543552"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1497,7 +1490,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="275602224"/>
+        <c:axId val="251542992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,12 +1636,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275602784"/>
+        <c:crossAx val="251543552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="275602784"/>
+        <c:axId val="251543552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,7 +1759,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275602224"/>
+        <c:crossAx val="251542992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1855,7 +1848,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1968,11 +1960,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="275605584"/>
-        <c:axId val="275606144"/>
+        <c:axId val="251546352"/>
+        <c:axId val="251546912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="275605584"/>
+        <c:axId val="251546352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2023,7 +2015,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2090,12 +2081,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275606144"/>
+        <c:crossAx val="251546912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="275606144"/>
+        <c:axId val="251546912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2149,7 +2140,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2216,7 +2206,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275605584"/>
+        <c:crossAx val="251546352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2419,11 +2409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276126384"/>
-        <c:axId val="276126944"/>
+        <c:axId val="251549152"/>
+        <c:axId val="335895200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276126384"/>
+        <c:axId val="251549152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2541,12 +2531,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276126944"/>
+        <c:crossAx val="335895200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276126944"/>
+        <c:axId val="335895200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2664,7 +2654,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276126384"/>
+        <c:crossAx val="251549152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2936,11 +2926,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276129184"/>
-        <c:axId val="276129744"/>
+        <c:axId val="335897440"/>
+        <c:axId val="335898000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276129184"/>
+        <c:axId val="335897440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3058,12 +3048,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276129744"/>
+        <c:crossAx val="335898000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276129744"/>
+        <c:axId val="335898000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3177,7 +3167,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276129184"/>
+        <c:crossAx val="335897440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3449,8 +3439,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276132544"/>
-        <c:axId val="276133104"/>
+        <c:axId val="335900800"/>
+        <c:axId val="335901360"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3641,7 +3631,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276132544"/>
+        <c:axId val="335900800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3759,12 +3749,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276133104"/>
+        <c:crossAx val="335901360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276133104"/>
+        <c:axId val="335901360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3877,7 +3867,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276132544"/>
+        <c:crossAx val="335900800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3966,7 +3956,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4059,8 +4048,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="349008352"/>
-        <c:axId val="349010592"/>
+        <c:axId val="335998256"/>
+        <c:axId val="335998816"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4127,7 +4116,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="349008352"/>
+        <c:axId val="335998256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4169,7 +4158,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349010592"/>
+        <c:crossAx val="335998816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4177,7 +4166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349010592"/>
+        <c:axId val="335998816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4228,7 +4217,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349008352"/>
+        <c:crossAx val="335998256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4317,7 +4306,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4410,8 +4398,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="470480272"/>
-        <c:axId val="349586880"/>
+        <c:axId val="336001616"/>
+        <c:axId val="336002176"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4478,7 +4466,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="470480272"/>
+        <c:axId val="336001616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4520,7 +4508,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349586880"/>
+        <c:crossAx val="336002176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4528,7 +4516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349586880"/>
+        <c:axId val="336002176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4579,7 +4567,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470480272"/>
+        <c:crossAx val="336001616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4782,11 +4770,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="473666864"/>
-        <c:axId val="473663504"/>
+        <c:axId val="335754384"/>
+        <c:axId val="335754944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="473666864"/>
+        <c:axId val="335754384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4829,7 +4817,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473663504"/>
+        <c:crossAx val="335754944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4837,7 +4825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="473663504"/>
+        <c:axId val="335754944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4888,7 +4876,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473666864"/>
+        <c:crossAx val="335754384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11479,13 +11467,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -11499,7 +11487,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>7</v>
@@ -12238,10 +12226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12250,11 +12238,10 @@
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="26.375" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="22.375" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -12265,9 +12252,8 @@
         <v>3</v>
       </c>
       <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -12281,13 +12267,10 @@
         <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="6"/>
       <c r="B3" s="8">
         <v>0.7</v>
@@ -12299,13 +12282,10 @@
         <v>0.149879678413879</v>
       </c>
       <c r="E3" s="8">
-        <v>0.149894040581977</v>
-      </c>
-      <c r="F3" s="8">
         <v>-5.0933375710002199E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="6"/>
       <c r="B4" s="8">
         <v>0.7</v>
@@ -12316,12 +12296,11 @@
       <c r="D4" s="8">
         <v>0.149879678413879</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="8">
+      <c r="E4" s="8">
         <v>-5.0933375709802699E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="6"/>
       <c r="B5" s="8">
         <v>0.7</v>
@@ -12332,10 +12311,11 @@
       <c r="D5" s="8">
         <v>0.149879678413879</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="E5" s="8">
+        <v>-5.0933375710048398E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="6"/>
       <c r="B6" s="6">
         <v>0.85</v>
@@ -12346,10 +12326,11 @@
       <c r="D6" s="8">
         <v>0.15755028460432899</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="E6" s="8">
+        <v>-5.04511633798903E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="6"/>
       <c r="B7" s="6">
         <v>0.85</v>
@@ -12361,13 +12342,10 @@
         <v>0.15755028460432899</v>
       </c>
       <c r="E7" s="8">
-        <v>0.15755588103264501</v>
-      </c>
-      <c r="F7" s="8">
         <v>-5.0451163380993203E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="6"/>
       <c r="B8" s="6">
         <v>0.85</v>
@@ -12378,10 +12356,11 @@
       <c r="D8" s="8">
         <v>0.15755028460432899</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="E8" s="8">
+        <v>-5.0451163381186902E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="6"/>
       <c r="B9" s="6">
         <v>0.9</v>
@@ -12392,10 +12371,11 @@
       <c r="D9" s="8">
         <v>0.159741542580674</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="E9" s="8">
+        <v>-5.0288965681501901E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="6"/>
       <c r="B10" s="6">
         <v>0.9</v>
@@ -12406,12 +12386,11 @@
       <c r="D10" s="8">
         <v>0.15974335604540901</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8">
+      <c r="E10" s="8">
         <v>-5.0288965677241497E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="6"/>
       <c r="B11" s="6">
         <v>0.9</v>
@@ -12422,8 +12401,9 @@
       <c r="D11" s="8">
         <v>0.15974335604540901</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="8">
+        <v>-5.0288965678785699E-2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -12436,7 +12416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -12480,7 +12460,7 @@
         <v>-8.6920912663615503E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -12613,7 +12593,7 @@
         <v>7.2824815996142794E-2</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -12699,7 +12679,7 @@
         <v>1.06565678427087E-2</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.15">
@@ -12876,7 +12856,7 @@
         <v>-2.6042330806943698E-2</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.15">
@@ -12930,7 +12910,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="G20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -13002,7 +12982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
+    <sheetView topLeftCell="E30" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G27"/>
     </sheetView>
   </sheetViews>
@@ -13010,22 +12990,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -13284,10 +13264,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
         <v>30</v>
-      </c>
-      <c r="G23" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -13324,13 +13304,13 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
         <v>27</v>
-      </c>
-      <c r="C36" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -13554,10 +13534,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -13594,10 +13574,10 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
         <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
some experiments results update
</commit_message>
<xml_diff>
--- a/data/experiments/results.xlsx
+++ b/data/experiments/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="10470" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="datarank" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +195,14 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,6 +247,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,11 +490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="250175264"/>
-        <c:axId val="250175824"/>
+        <c:axId val="254006992"/>
+        <c:axId val="254007552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="250175264"/>
+        <c:axId val="254006992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,12 +606,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250175824"/>
+        <c:crossAx val="254007552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="250175824"/>
+        <c:axId val="254007552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +728,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250175264"/>
+        <c:crossAx val="254006992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -806,7 +817,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -920,11 +930,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="335757184"/>
-        <c:axId val="335757744"/>
+        <c:axId val="351051712"/>
+        <c:axId val="351052272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="335757184"/>
+        <c:axId val="351051712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,7 +977,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335757744"/>
+        <c:crossAx val="351052272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -975,7 +985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335757744"/>
+        <c:axId val="351052272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1026,7 +1036,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335757184"/>
+        <c:crossAx val="351051712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,7 +1100,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1298,8 +1307,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251542992"/>
-        <c:axId val="251543552"/>
+        <c:axId val="254010352"/>
+        <c:axId val="254008672"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1490,7 +1499,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251542992"/>
+        <c:axId val="254010352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,7 +1564,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1636,12 +1644,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251543552"/>
+        <c:crossAx val="254008672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251543552"/>
+        <c:axId val="254008672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,7 +1700,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1759,7 +1766,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251542992"/>
+        <c:crossAx val="254010352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1960,11 +1967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251546352"/>
-        <c:axId val="251546912"/>
+        <c:axId val="254010912"/>
+        <c:axId val="254753568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251546352"/>
+        <c:axId val="254010912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,12 +2088,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251546912"/>
+        <c:crossAx val="254753568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251546912"/>
+        <c:axId val="254753568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2206,7 +2213,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251546352"/>
+        <c:crossAx val="254010912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2296,7 +2303,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2409,11 +2415,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251549152"/>
-        <c:axId val="335895200"/>
+        <c:axId val="254756368"/>
+        <c:axId val="254756928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251549152"/>
+        <c:axId val="254756368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2464,7 +2470,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2531,12 +2536,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335895200"/>
+        <c:crossAx val="254756928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335895200"/>
+        <c:axId val="254756928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2587,7 +2592,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2654,7 +2658,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251549152"/>
+        <c:crossAx val="254756368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2718,7 +2722,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2926,11 +2929,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335897440"/>
-        <c:axId val="335898000"/>
+        <c:axId val="350760112"/>
+        <c:axId val="350760672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335897440"/>
+        <c:axId val="350760112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2981,7 +2984,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3048,12 +3050,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335898000"/>
+        <c:crossAx val="350760672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335898000"/>
+        <c:axId val="350760672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3100,7 +3102,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3167,7 +3168,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335897440"/>
+        <c:crossAx val="350760112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3231,7 +3232,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3439,8 +3439,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335900800"/>
-        <c:axId val="335901360"/>
+        <c:axId val="350763472"/>
+        <c:axId val="350764032"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3631,7 +3631,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335900800"/>
+        <c:axId val="350763472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3682,7 +3682,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3749,12 +3748,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335901360"/>
+        <c:crossAx val="350764032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335901360"/>
+        <c:axId val="350764032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3800,7 +3799,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3867,7 +3865,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335900800"/>
+        <c:crossAx val="350763472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4048,8 +4046,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="335998256"/>
-        <c:axId val="335998816"/>
+        <c:axId val="350766832"/>
+        <c:axId val="350767392"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4116,7 +4114,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="335998256"/>
+        <c:axId val="350766832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4158,7 +4156,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335998816"/>
+        <c:crossAx val="350767392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4166,7 +4164,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335998816"/>
+        <c:axId val="350767392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4217,7 +4215,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335998256"/>
+        <c:crossAx val="350766832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4398,8 +4396,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="336001616"/>
-        <c:axId val="336002176"/>
+        <c:axId val="351221856"/>
+        <c:axId val="351222416"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4466,7 +4464,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="336001616"/>
+        <c:axId val="351221856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4508,7 +4506,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="336002176"/>
+        <c:crossAx val="351222416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4516,7 +4514,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="336002176"/>
+        <c:axId val="351222416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4567,7 +4565,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="336001616"/>
+        <c:crossAx val="351221856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4656,7 +4654,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4770,11 +4767,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="335754384"/>
-        <c:axId val="335754944"/>
+        <c:axId val="351224656"/>
+        <c:axId val="351225216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="335754384"/>
+        <c:axId val="351224656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4817,7 +4814,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335754944"/>
+        <c:crossAx val="351225216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4825,7 +4822,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335754944"/>
+        <c:axId val="351225216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4876,7 +4873,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335754384"/>
+        <c:crossAx val="351224656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11449,10 +11446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11461,7 +11458,7 @@
     <col min="2" max="2" width="17.75" customWidth="1"/>
     <col min="3" max="3" width="19.625" customWidth="1"/>
     <col min="4" max="4" width="14.75" customWidth="1"/>
-    <col min="5" max="5" width="22.25" customWidth="1"/>
+    <col min="5" max="5" width="22.25" style="6" customWidth="1"/>
     <col min="6" max="6" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11506,15 +11503,13 @@
       <c r="C3" s="7">
         <v>0.25</v>
       </c>
-      <c r="D3" s="7">
-        <v>0.1</v>
+      <c r="D3" s="9">
+        <v>0.01</v>
       </c>
       <c r="E3" s="8">
-        <v>0.16732515469086501</v>
-      </c>
-      <c r="F3" s="8">
-        <v>-8.6920912663614202E-4</v>
-      </c>
+        <v>-6.3732852200766799E-2</v>
+      </c>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
@@ -11526,15 +11521,13 @@
       <c r="C4" s="7">
         <v>0.25</v>
       </c>
-      <c r="D4" s="7">
-        <v>0.2</v>
+      <c r="D4" s="9">
+        <v>0.05</v>
       </c>
       <c r="E4" s="8">
-        <v>0.167786226660851</v>
-      </c>
-      <c r="F4" s="8">
-        <v>-8.6920912663616099E-4</v>
-      </c>
+        <v>4.59159690742513E-2</v>
+      </c>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
@@ -11544,16 +11537,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="7">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D5" s="7">
         <v>0.1</v>
       </c>
       <c r="E5" s="8">
-        <v>0.10612083534611499</v>
+        <v>0.16732515469086501</v>
       </c>
       <c r="F5" s="8">
-        <v>-8.2981553194450396E-3</v>
+        <v>-8.6920912663614202E-4</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -11564,16 +11557,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="7">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D6" s="7">
         <v>0.2</v>
       </c>
       <c r="E6" s="8">
-        <v>0.105550667756504</v>
+        <v>0.167786226660851</v>
       </c>
       <c r="F6" s="8">
-        <v>-8.29815531944505E-3</v>
+        <v>-8.6920912663616099E-4</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -11581,48 +11574,43 @@
         <v>1</v>
       </c>
       <c r="B7" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0.1</v>
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.01</v>
       </c>
       <c r="E7" s="8">
-        <v>-0.138366130536939</v>
-      </c>
-      <c r="F7" s="8">
-        <f>0.0442791673085406</f>
-        <v>4.4279167308540597E-2</v>
-      </c>
+        <v>-6.8414149256397605E-2</v>
+      </c>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>1</v>
       </c>
       <c r="B8" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0.2</v>
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.05</v>
       </c>
       <c r="E8" s="8">
-        <v>-0.138366130536939</v>
-      </c>
-      <c r="F8" s="8">
-        <v>4.4279167308540701E-2</v>
-      </c>
+        <v>1.0946941749575299E-2</v>
+      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>1</v>
       </c>
       <c r="B9" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9" s="7">
         <v>0.5</v>
@@ -11631,10 +11619,10 @@
         <v>0.1</v>
       </c>
       <c r="E9" s="8">
-        <v>-0.16680670635632</v>
+        <v>0.10612083534611499</v>
       </c>
       <c r="F9" s="8">
-        <v>3.4809877951280703E-2</v>
+        <v>-8.2981553194450396E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -11642,7 +11630,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="7">
         <v>0.5</v>
@@ -11651,10 +11639,10 @@
         <v>0.2</v>
       </c>
       <c r="E10" s="8">
-        <v>-0.16680670635632</v>
+        <v>0.105550667756504</v>
       </c>
       <c r="F10" s="8">
-        <v>3.4809877951280703E-2</v>
+        <v>-8.29815531944505E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -11662,59 +11650,56 @@
         <v>1</v>
       </c>
       <c r="B11" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C11" s="7">
         <v>0.25</v>
       </c>
-      <c r="D11" s="7">
-        <v>0.1</v>
+      <c r="D11" s="9">
+        <v>0.01</v>
       </c>
       <c r="E11" s="8">
-        <v>-0.20064574260235299</v>
-      </c>
-      <c r="F11" s="8">
-        <v>9.1606957031747593E-2</v>
-      </c>
+        <v>-0.170583522798298</v>
+      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>1</v>
       </c>
       <c r="B12" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C12" s="7">
         <v>0.25</v>
       </c>
-      <c r="D12" s="7">
-        <v>0.2</v>
+      <c r="D12" s="9">
+        <v>0.05</v>
       </c>
       <c r="E12" s="8">
-        <v>-0.20064600597264301</v>
-      </c>
-      <c r="F12" s="8">
-        <v>9.1606957031747496E-2</v>
-      </c>
+        <v>-0.170583522798298</v>
+      </c>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>1</v>
       </c>
       <c r="B13" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C13" s="7">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D13" s="7">
         <v>0.1</v>
       </c>
       <c r="E13" s="8">
-        <v>-0.22937851504088699</v>
+        <v>-0.138366130536939</v>
       </c>
       <c r="F13" s="8">
-        <v>7.2824815996142503E-2</v>
+        <f>0.0442791673085406</f>
+        <v>4.4279167308540597E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -11722,67 +11707,63 @@
         <v>1</v>
       </c>
       <c r="B14" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C14" s="7">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D14" s="7">
         <v>0.2</v>
       </c>
       <c r="E14" s="8">
-        <v>-0.22937848981526701</v>
+        <v>-0.138366130536939</v>
       </c>
       <c r="F14" s="8">
-        <v>7.2824815996142503E-2</v>
+        <v>4.4279167308540701E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7">
         <v>5</v>
       </c>
-      <c r="B15" s="7">
-        <v>1</v>
-      </c>
       <c r="C15" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0.1</v>
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.01</v>
       </c>
       <c r="E15" s="8">
-        <v>0.15834969330333901</v>
-      </c>
-      <c r="F15" s="8">
-        <v>-2.92391655578099E-2</v>
-      </c>
+        <v>-0.17490106308836301</v>
+      </c>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7">
         <v>5</v>
       </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
       <c r="C16" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.2</v>
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.05</v>
       </c>
       <c r="E16" s="8">
-        <v>0.15824305717044701</v>
-      </c>
-      <c r="F16" s="8">
-        <v>-2.92411016889653E-2</v>
-      </c>
+        <v>-0.17490106308836301</v>
+      </c>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7">
         <v>5</v>
-      </c>
-      <c r="B17" s="7">
-        <v>1</v>
       </c>
       <c r="C17" s="7">
         <v>0.5</v>
@@ -11791,18 +11772,18 @@
         <v>0.1</v>
       </c>
       <c r="E17" s="8">
-        <v>0.12893431014342599</v>
+        <v>-0.16680670635632</v>
       </c>
       <c r="F17" s="8">
-        <v>-2.84339125983748E-2</v>
+        <v>3.4809877951280703E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="7">
+        <v>1</v>
+      </c>
+      <c r="B18" s="7">
         <v>5</v>
-      </c>
-      <c r="B18" s="7">
-        <v>1</v>
       </c>
       <c r="C18" s="7">
         <v>0.5</v>
@@ -11811,135 +11792,127 @@
         <v>0.2</v>
       </c>
       <c r="E18" s="8">
-        <v>0.12867122132689901</v>
+        <v>-0.16680670635632</v>
       </c>
       <c r="F18" s="8">
-        <v>-2.84339125983749E-2</v>
+        <v>3.4809877951280703E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B19" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C19" s="7">
         <v>0.25</v>
       </c>
-      <c r="D19" s="7">
-        <v>0.1</v>
+      <c r="D19" s="9">
+        <v>0.01</v>
       </c>
       <c r="E19" s="8">
-        <v>5.3416589194425601E-2</v>
-      </c>
-      <c r="F19" s="8">
-        <v>8.7863724707500802E-3</v>
-      </c>
+        <v>-0.23319416565937501</v>
+      </c>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B20" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C20" s="7">
         <v>0.25</v>
       </c>
-      <c r="D20" s="7">
-        <v>0.2</v>
+      <c r="D20" s="9">
+        <v>0.05</v>
       </c>
       <c r="E20" s="8">
-        <v>5.3416589194425802E-2</v>
-      </c>
-      <c r="F20" s="8">
-        <v>8.7845794012064299E-3</v>
-      </c>
+        <v>-0.23319416565937501</v>
+      </c>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B21" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C21" s="7">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D21" s="7">
         <v>0.1</v>
       </c>
       <c r="E21" s="8">
-        <v>-7.0282122882539599E-2</v>
+        <v>-0.20064574260235299</v>
       </c>
       <c r="F21" s="8">
-        <v>1.0656567842708801E-2</v>
+        <v>9.1606957031747593E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B22" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C22" s="7">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D22" s="7">
         <v>0.2</v>
       </c>
       <c r="E22" s="8">
-        <v>-7.0282122882539599E-2</v>
+        <v>-0.20064600597264301</v>
       </c>
       <c r="F22" s="8">
-        <v>1.0656567842708801E-2</v>
+        <v>9.1606957031747496E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23" s="7">
         <v>20</v>
       </c>
       <c r="C23" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0.1</v>
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.01</v>
       </c>
       <c r="E23" s="8">
-        <v>2.2160466980396198E-2</v>
-      </c>
-      <c r="F23" s="8">
-        <v>3.7713533408709702E-3</v>
-      </c>
+        <v>-0.23735532343278001</v>
+      </c>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B24" s="7">
         <v>20</v>
       </c>
       <c r="C24" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0.2</v>
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.05</v>
       </c>
       <c r="E24" s="8">
-        <v>2.21598482080612E-2</v>
-      </c>
-      <c r="F24" s="8">
-        <v>3.7713533408709598E-3</v>
-      </c>
+        <v>-0.23735532343278001</v>
+      </c>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B25" s="7">
         <v>20</v>
@@ -11951,15 +11924,15 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="8">
-        <v>-0.12035305807387001</v>
+        <v>-0.22937851504088699</v>
       </c>
       <c r="F25" s="8">
-        <v>8.8511386950287096E-3</v>
+        <v>7.2824815996142503E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B26" s="7">
         <v>20</v>
@@ -11971,35 +11944,23 @@
         <v>0.2</v>
       </c>
       <c r="E26" s="8">
-        <v>-0.120353249554302</v>
+        <v>-0.22937848981526701</v>
       </c>
       <c r="F26" s="8">
-        <v>8.8511386950288293E-3</v>
+        <v>7.2824815996142503E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A27" s="7">
-        <v>20</v>
-      </c>
-      <c r="B27" s="7">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E27" s="8">
-        <v>0.15313922148498199</v>
-      </c>
-      <c r="F27" s="8">
-        <v>-5.88753318492405E-2</v>
-      </c>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B28" s="7">
         <v>1</v>
@@ -12007,213 +11968,913 @@
       <c r="C28" s="7">
         <v>0.25</v>
       </c>
-      <c r="D28" s="7">
-        <v>0.2</v>
+      <c r="D28" s="9">
+        <v>0.01</v>
       </c>
       <c r="E28" s="8">
-        <v>0.15313922148498199</v>
-      </c>
-      <c r="F28" s="8">
-        <v>-5.8875331849240597E-2</v>
-      </c>
+        <v>9.4118431815529605E-2</v>
+      </c>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B29" s="7">
         <v>1</v>
       </c>
       <c r="C29" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0.1</v>
+        <v>0.25</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.05</v>
       </c>
       <c r="E29" s="8">
-        <v>0.13266509586470199</v>
-      </c>
-      <c r="F29" s="8">
-        <v>-5.2623625398156099E-2</v>
-      </c>
+        <v>9.4118431815529702E-2</v>
+      </c>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B30" s="7">
         <v>1</v>
       </c>
       <c r="C30" s="7">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D30" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E30" s="8">
-        <v>0.13266509586470199</v>
+        <v>0.15834969330333901</v>
       </c>
       <c r="F30" s="8">
-        <v>-5.2623625398156099E-2</v>
+        <v>-2.92391655578099E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B31" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C31" s="7">
         <v>0.25</v>
       </c>
       <c r="D31" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E31" s="8">
-        <v>0.108027884460389</v>
+        <v>0.15824305717044701</v>
       </c>
       <c r="F31" s="8">
-        <v>-3.6518484126942898E-2</v>
+        <v>-2.92411016889653E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B32" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C32" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D32" s="7">
-        <v>0.2</v>
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.01</v>
       </c>
       <c r="E32" s="8">
-        <v>0.108027884460389</v>
-      </c>
-      <c r="F32" s="8">
-        <v>-3.6518484126942898E-2</v>
-      </c>
+        <v>8.0078535146042296E-2</v>
+      </c>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B33" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C33" s="7">
         <v>0.5</v>
       </c>
-      <c r="D33" s="7">
-        <v>0.1</v>
+      <c r="D33" s="9">
+        <v>0.05</v>
       </c>
       <c r="E33" s="8">
-        <v>2.3965435250042199E-2</v>
-      </c>
-      <c r="F33" s="8">
-        <v>-2.6042330806943799E-2</v>
-      </c>
+        <v>8.0078535146042296E-2</v>
+      </c>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B34" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C34" s="7">
         <v>0.5</v>
       </c>
       <c r="D34" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E34" s="8">
-        <v>2.3965435250042199E-2</v>
+        <v>0.12893431014342599</v>
       </c>
       <c r="F34" s="8">
-        <v>-2.6063045074091799E-2</v>
+        <v>-2.84339125983748E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B35" s="7">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C35" s="7">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D35" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E35" s="8">
-        <v>9.1612494841683406E-2</v>
+        <v>0.12867122132689901</v>
       </c>
       <c r="F35" s="8">
-        <v>-4.2581416135986698E-2</v>
+        <v>-2.84339125983749E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B36" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C36" s="7">
         <v>0.25</v>
       </c>
-      <c r="D36" s="7">
-        <v>0.2</v>
+      <c r="D36" s="9">
+        <v>0.01</v>
       </c>
       <c r="E36" s="8">
-        <v>9.1614115691380504E-2</v>
-      </c>
-      <c r="F36" s="8">
-        <v>-4.2581416135986802E-2</v>
-      </c>
+        <v>-4.4793364376875297E-2</v>
+      </c>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B37" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C37" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D37" s="7">
-        <v>0.1</v>
+        <v>0.25</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0.05</v>
       </c>
       <c r="E37" s="8">
-        <v>-9.2409072476452997E-3</v>
-      </c>
-      <c r="F37" s="8">
-        <v>-4.13107001371062E-2</v>
-      </c>
+        <v>-4.4793364376875297E-2</v>
+      </c>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="7">
+        <v>5</v>
+      </c>
+      <c r="B38" s="7">
+        <v>5</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E38" s="8">
+        <v>5.3416589194425601E-2</v>
+      </c>
+      <c r="F38" s="8">
+        <v>8.7863724707500802E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A39" s="7">
+        <v>5</v>
+      </c>
+      <c r="B39" s="7">
+        <v>5</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E39" s="8">
+        <v>5.3416589194425802E-2</v>
+      </c>
+      <c r="F39" s="8">
+        <v>8.7845794012064299E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A40" s="7">
+        <v>5</v>
+      </c>
+      <c r="B40" s="7">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E40" s="8">
+        <v>-0.11320154713019701</v>
+      </c>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A41" s="7">
+        <v>5</v>
+      </c>
+      <c r="B41" s="7">
+        <v>5</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D41" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E41" s="8">
+        <v>-0.11320154713019701</v>
+      </c>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A42" s="7">
+        <v>5</v>
+      </c>
+      <c r="B42" s="7">
+        <v>5</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E42" s="8">
+        <v>-7.0282122882539599E-2</v>
+      </c>
+      <c r="F42" s="8">
+        <v>1.0656567842708801E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A43" s="7">
+        <v>5</v>
+      </c>
+      <c r="B43" s="7">
+        <v>5</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E43" s="8">
+        <v>-7.0282122882539599E-2</v>
+      </c>
+      <c r="F43" s="8">
+        <v>1.0656567842708801E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A44" s="7">
+        <v>5</v>
+      </c>
+      <c r="B44" s="7">
         <v>20</v>
       </c>
-      <c r="B38" s="7">
+      <c r="C44" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E44" s="8">
+        <v>-8.4881321751472602E-2</v>
+      </c>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A45" s="7">
+        <v>5</v>
+      </c>
+      <c r="B45" s="7">
         <v>20</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C45" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E45" s="8">
+        <v>-8.4881321751472602E-2</v>
+      </c>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A46" s="7">
+        <v>5</v>
+      </c>
+      <c r="B46" s="7">
+        <v>20</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E46" s="8">
+        <v>2.2160466980396198E-2</v>
+      </c>
+      <c r="F46" s="8">
+        <v>3.7713533408709702E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A47" s="7">
+        <v>5</v>
+      </c>
+      <c r="B47" s="7">
+        <v>20</v>
+      </c>
+      <c r="C47" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D47" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E47" s="8">
+        <v>2.21598482080612E-2</v>
+      </c>
+      <c r="F47" s="8">
+        <v>3.7713533408709598E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A48" s="7">
+        <v>5</v>
+      </c>
+      <c r="B48" s="7">
+        <v>20</v>
+      </c>
+      <c r="C48" s="7">
         <v>0.5</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D48" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E48" s="8">
+        <v>-0.165584851919304</v>
+      </c>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A49" s="7">
+        <v>5</v>
+      </c>
+      <c r="B49" s="7">
+        <v>20</v>
+      </c>
+      <c r="C49" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E49" s="8">
+        <v>-0.165584851919304</v>
+      </c>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A50" s="7">
+        <v>5</v>
+      </c>
+      <c r="B50" s="7">
+        <v>20</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E50" s="8">
+        <v>-0.12035305807387001</v>
+      </c>
+      <c r="F50" s="8">
+        <v>8.8511386950287096E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A51" s="7">
+        <v>5</v>
+      </c>
+      <c r="B51" s="7">
+        <v>20</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D51" s="7">
         <v>0.2</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E51" s="8">
+        <v>-0.120353249554302</v>
+      </c>
+      <c r="F51" s="8">
+        <v>8.8511386950288293E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A53" s="7">
+        <v>20</v>
+      </c>
+      <c r="B53" s="7">
+        <v>1</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E53" s="8">
+        <v>0.14743629252229701</v>
+      </c>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A54" s="7">
+        <v>20</v>
+      </c>
+      <c r="B54" s="7">
+        <v>1</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D54" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E54" s="8">
+        <v>0.14743629252229701</v>
+      </c>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A55" s="7">
+        <v>20</v>
+      </c>
+      <c r="B55" s="7">
+        <v>1</v>
+      </c>
+      <c r="C55" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E55" s="8">
+        <v>0.15313922148498199</v>
+      </c>
+      <c r="F55" s="8">
+        <v>-5.88753318492405E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A56" s="7">
+        <v>20</v>
+      </c>
+      <c r="B56" s="7">
+        <v>1</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E56" s="8">
+        <v>0.15313922148498199</v>
+      </c>
+      <c r="F56" s="8">
+        <v>-5.8875331849240597E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A57" s="7">
+        <v>20</v>
+      </c>
+      <c r="B57" s="7">
+        <v>1</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D57" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E57" s="8">
+        <v>0.103763087815315</v>
+      </c>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A58" s="7">
+        <v>20</v>
+      </c>
+      <c r="B58" s="7">
+        <v>1</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E58" s="8">
+        <v>0.103763087815315</v>
+      </c>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A59" s="7">
+        <v>20</v>
+      </c>
+      <c r="B59" s="7">
+        <v>1</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E59" s="8">
+        <v>0.13266509586470199</v>
+      </c>
+      <c r="F59" s="8">
+        <v>-5.2623625398156099E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A60" s="7">
+        <v>20</v>
+      </c>
+      <c r="B60" s="7">
+        <v>1</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D60" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E60" s="8">
+        <v>0.13266509586470199</v>
+      </c>
+      <c r="F60" s="8">
+        <v>-5.2623625398156099E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A61" s="7">
+        <v>20</v>
+      </c>
+      <c r="B61" s="7">
+        <v>5</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D61" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E61" s="8">
+        <v>9.8642849217424694E-2</v>
+      </c>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A62" s="7">
+        <v>20</v>
+      </c>
+      <c r="B62" s="7">
+        <v>5</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D62" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E62" s="8">
+        <v>9.8642849217424597E-2</v>
+      </c>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A63" s="7">
+        <v>20</v>
+      </c>
+      <c r="B63" s="7">
+        <v>5</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D63" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E63" s="8">
+        <v>0.108027884460389</v>
+      </c>
+      <c r="F63" s="8">
+        <v>-3.6518484126942898E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A64" s="7">
+        <v>20</v>
+      </c>
+      <c r="B64" s="7">
+        <v>5</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D64" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E64" s="8">
+        <v>0.108027884460389</v>
+      </c>
+      <c r="F64" s="8">
+        <v>-3.6518484126942898E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A65" s="7">
+        <v>20</v>
+      </c>
+      <c r="B65" s="7">
+        <v>5</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E65" s="8">
+        <v>-1.8755832844895199E-2</v>
+      </c>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A66" s="7">
+        <v>20</v>
+      </c>
+      <c r="B66" s="7">
+        <v>5</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E66" s="8">
+        <v>-1.8755832844895199E-2</v>
+      </c>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A67" s="7">
+        <v>20</v>
+      </c>
+      <c r="B67" s="7">
+        <v>5</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E67" s="8">
+        <v>2.3965435250042199E-2</v>
+      </c>
+      <c r="F67" s="8">
+        <v>-2.6042330806943799E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A68" s="7">
+        <v>20</v>
+      </c>
+      <c r="B68" s="7">
+        <v>5</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E68" s="8">
+        <v>2.3965435250042199E-2</v>
+      </c>
+      <c r="F68" s="8">
+        <v>-2.6063045074091799E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A69" s="7">
+        <v>20</v>
+      </c>
+      <c r="B69" s="7">
+        <v>20</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D69" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E69" s="8">
+        <v>8.1108723348584599E-2</v>
+      </c>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A70" s="7">
+        <v>20</v>
+      </c>
+      <c r="B70" s="7">
+        <v>20</v>
+      </c>
+      <c r="C70" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D70" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E70" s="8">
+        <v>8.1108723348584794E-2</v>
+      </c>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A71" s="7">
+        <v>20</v>
+      </c>
+      <c r="B71" s="7">
+        <v>20</v>
+      </c>
+      <c r="C71" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D71" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E71" s="8">
+        <v>9.1612494841683406E-2</v>
+      </c>
+      <c r="F71" s="8">
+        <v>-4.2581416135986698E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A72" s="7">
+        <v>20</v>
+      </c>
+      <c r="B72" s="7">
+        <v>20</v>
+      </c>
+      <c r="C72" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D72" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E72" s="8">
+        <v>9.1614115691380504E-2</v>
+      </c>
+      <c r="F72" s="8">
+        <v>-4.2581416135986802E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A73" s="7">
+        <v>20</v>
+      </c>
+      <c r="B73" s="7">
+        <v>20</v>
+      </c>
+      <c r="C73" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D73" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E73" s="8">
+        <v>-5.5297737433492901E-2</v>
+      </c>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A74" s="7">
+        <v>20</v>
+      </c>
+      <c r="B74" s="7">
+        <v>20</v>
+      </c>
+      <c r="C74" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D74" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E74" s="8">
+        <v>-5.5297737433492797E-2</v>
+      </c>
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A75" s="7">
+        <v>20</v>
+      </c>
+      <c r="B75" s="7">
+        <v>20</v>
+      </c>
+      <c r="C75" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D75" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E75" s="8">
+        <v>-9.2409072476452997E-3</v>
+      </c>
+      <c r="F75" s="8">
+        <v>-4.13107001371062E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A76" s="7">
+        <v>20</v>
+      </c>
+      <c r="B76" s="7">
+        <v>20</v>
+      </c>
+      <c r="C76" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D76" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E76" s="8">
         <v>-9.2410588069189708E-3</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F76" s="8">
         <v>-4.1321897718647402E-2</v>
       </c>
     </row>
@@ -12228,7 +12889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update datarank v2 results
</commit_message>
<xml_diff>
--- a/data/experiments/results.xlsx
+++ b/data/experiments/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10470" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="11400" yWindow="105" windowWidth="14805" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="datarank" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -224,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -250,6 +256,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,11 +499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="254006992"/>
-        <c:axId val="254007552"/>
+        <c:axId val="144737216"/>
+        <c:axId val="144737776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254006992"/>
+        <c:axId val="144737216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,12 +615,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254007552"/>
+        <c:crossAx val="144737776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="254007552"/>
+        <c:axId val="144737776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +737,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254006992"/>
+        <c:crossAx val="144737216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -930,11 +939,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="351051712"/>
-        <c:axId val="351052272"/>
+        <c:axId val="146585168"/>
+        <c:axId val="146585728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="351051712"/>
+        <c:axId val="146585168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +986,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351052272"/>
+        <c:crossAx val="146585728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="351052272"/>
+        <c:axId val="146585728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +1045,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351051712"/>
+        <c:crossAx val="146585168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1307,8 +1316,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="254010352"/>
-        <c:axId val="254008672"/>
+        <c:axId val="144740576"/>
+        <c:axId val="144741136"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1499,7 +1508,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254010352"/>
+        <c:axId val="144740576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,12 +1653,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254008672"/>
+        <c:crossAx val="144741136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="254008672"/>
+        <c:axId val="144741136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,7 +1775,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254010352"/>
+        <c:crossAx val="144740576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1967,11 +1976,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="254010912"/>
-        <c:axId val="254753568"/>
+        <c:axId val="145910528"/>
+        <c:axId val="145911088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254010912"/>
+        <c:axId val="145910528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,12 +2097,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254753568"/>
+        <c:crossAx val="145911088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="254753568"/>
+        <c:axId val="145911088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2222,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254010912"/>
+        <c:crossAx val="145910528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2415,11 +2424,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="254756368"/>
-        <c:axId val="254756928"/>
+        <c:axId val="145913328"/>
+        <c:axId val="145913888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254756368"/>
+        <c:axId val="145913328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2536,12 +2545,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254756928"/>
+        <c:crossAx val="145913888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="254756928"/>
+        <c:axId val="145913888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2658,7 +2667,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254756368"/>
+        <c:crossAx val="145913328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2929,11 +2938,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="350760112"/>
-        <c:axId val="350760672"/>
+        <c:axId val="146720832"/>
+        <c:axId val="146721392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="350760112"/>
+        <c:axId val="146720832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3050,12 +3059,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350760672"/>
+        <c:crossAx val="146721392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350760672"/>
+        <c:axId val="146721392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,7 +3177,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350760112"/>
+        <c:crossAx val="146720832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3439,8 +3448,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="350763472"/>
-        <c:axId val="350764032"/>
+        <c:axId val="146724192"/>
+        <c:axId val="146724752"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3631,7 +3640,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="350763472"/>
+        <c:axId val="146724192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3748,12 +3757,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350764032"/>
+        <c:crossAx val="146724752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350764032"/>
+        <c:axId val="146724752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3865,7 +3874,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350763472"/>
+        <c:crossAx val="146724192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4046,8 +4055,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="350766832"/>
-        <c:axId val="350767392"/>
+        <c:axId val="146728112"/>
+        <c:axId val="146380880"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4114,7 +4123,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="350766832"/>
+        <c:axId val="146728112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4156,7 +4165,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350767392"/>
+        <c:crossAx val="146380880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4164,7 +4173,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350767392"/>
+        <c:axId val="146380880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4215,7 +4224,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350766832"/>
+        <c:crossAx val="146728112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4396,8 +4405,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="351221856"/>
-        <c:axId val="351222416"/>
+        <c:axId val="146383680"/>
+        <c:axId val="146384240"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4464,7 +4473,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="351221856"/>
+        <c:axId val="146383680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4506,7 +4515,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351222416"/>
+        <c:crossAx val="146384240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4514,7 +4523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="351222416"/>
+        <c:axId val="146384240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4565,7 +4574,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351221856"/>
+        <c:crossAx val="146383680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4767,11 +4776,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="351224656"/>
-        <c:axId val="351225216"/>
+        <c:axId val="146386480"/>
+        <c:axId val="146387040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="351224656"/>
+        <c:axId val="146386480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4814,7 +4823,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351225216"/>
+        <c:crossAx val="146387040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4822,7 +4831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="351225216"/>
+        <c:axId val="146387040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4873,7 +4882,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351224656"/>
+        <c:crossAx val="146386480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11446,10 +11455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -11459,7 +11468,7 @@
     <col min="3" max="3" width="19.625" customWidth="1"/>
     <col min="4" max="4" width="14.75" customWidth="1"/>
     <col min="5" max="5" width="22.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="26.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -11509,7 +11518,9 @@
       <c r="E3" s="8">
         <v>-6.3732852200766799E-2</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="8">
+        <v>-8.6920912663612999E-4</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
@@ -11527,7 +11538,9 @@
       <c r="E4" s="8">
         <v>4.59159690742513E-2</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="8">
+        <v>-8.6920912663614397E-4</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
@@ -11585,7 +11598,9 @@
       <c r="E7" s="8">
         <v>-6.8414149256397605E-2</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8">
+        <v>-8.29815531944505E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
@@ -11603,7 +11618,9 @@
       <c r="E8" s="8">
         <v>1.0946941749575299E-2</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <v>-8.29815531944505E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
@@ -11661,7 +11678,9 @@
       <c r="E11" s="8">
         <v>-0.170583522798298</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <v>4.4279167308540701E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
@@ -11679,7 +11698,9 @@
       <c r="E12" s="8">
         <v>-0.170583522798298</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8">
+        <v>4.4279167308540701E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
@@ -11738,7 +11759,9 @@
       <c r="E15" s="8">
         <v>-0.17490106308836301</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8">
+        <v>3.4809877951280703E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
@@ -11756,7 +11779,9 @@
       <c r="E16" s="8">
         <v>-0.17490106308836301</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8">
+        <v>3.4809877951280599E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
@@ -11814,7 +11839,9 @@
       <c r="E19" s="8">
         <v>-0.23319416565937501</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8">
+        <v>9.1606957031747496E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="7">
@@ -11832,7 +11859,9 @@
       <c r="E20" s="8">
         <v>-0.23319416565937501</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="8">
+        <v>9.1606957031747593E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="7">
@@ -11890,7 +11919,9 @@
       <c r="E23" s="8">
         <v>-0.23735532343278001</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8">
+        <v>7.2824815996142794E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="7">
@@ -11908,7 +11939,9 @@
       <c r="E24" s="8">
         <v>-0.23735532343278001</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8">
+        <v>7.2824815996142697E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="7">
@@ -11951,28 +11984,38 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="10">
+        <v>-0.23916289923186801</v>
+      </c>
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A28" s="7">
-        <v>5</v>
-      </c>
-      <c r="B28" s="7">
+      <c r="A28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D28" s="9">
+      <c r="B28" s="2">
+        <v>30</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="2">
         <v>0.01</v>
       </c>
-      <c r="E28" s="8">
-        <v>9.4118431815529605E-2</v>
+      <c r="E28" s="10">
+        <v>-0.24491303286643301</v>
       </c>
       <c r="F28" s="8"/>
     </row>
@@ -11987,12 +12030,14 @@
         <v>0.25</v>
       </c>
       <c r="D29" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E29" s="8">
-        <v>9.4118431815529702E-2</v>
-      </c>
-      <c r="F29" s="8"/>
+        <v>9.4118431815529605E-2</v>
+      </c>
+      <c r="F29" s="8">
+        <v>-2.92391655578099E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="7">
@@ -12004,14 +12049,14 @@
       <c r="C30" s="7">
         <v>0.25</v>
       </c>
-      <c r="D30" s="7">
-        <v>0.1</v>
+      <c r="D30" s="9">
+        <v>0.05</v>
       </c>
       <c r="E30" s="8">
-        <v>0.15834969330333901</v>
+        <v>9.4118431815529702E-2</v>
       </c>
       <c r="F30" s="8">
-        <v>-2.92391655578099E-2</v>
+        <v>-2.92411016889653E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12025,13 +12070,13 @@
         <v>0.25</v>
       </c>
       <c r="D31" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E31" s="8">
-        <v>0.15824305717044701</v>
+        <v>0.15834969330333901</v>
       </c>
       <c r="F31" s="8">
-        <v>-2.92411016889653E-2</v>
+        <v>-2.92391655578099E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12042,15 +12087,17 @@
         <v>1</v>
       </c>
       <c r="C32" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0.01</v>
+        <v>0.25</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0.2</v>
       </c>
       <c r="E32" s="8">
-        <v>8.0078535146042296E-2</v>
-      </c>
-      <c r="F32" s="8"/>
+        <v>0.15824305717044701</v>
+      </c>
+      <c r="F32" s="8">
+        <v>-2.92411016889653E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="7">
@@ -12063,12 +12110,14 @@
         <v>0.5</v>
       </c>
       <c r="D33" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E33" s="8">
         <v>8.0078535146042296E-2</v>
       </c>
-      <c r="F33" s="8"/>
+      <c r="F33" s="8">
+        <v>-2.84339125983748E-2</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="7">
@@ -12080,14 +12129,14 @@
       <c r="C34" s="7">
         <v>0.5</v>
       </c>
-      <c r="D34" s="7">
-        <v>0.1</v>
+      <c r="D34" s="9">
+        <v>0.05</v>
       </c>
       <c r="E34" s="8">
-        <v>0.12893431014342599</v>
+        <v>8.0078535146042296E-2</v>
       </c>
       <c r="F34" s="8">
-        <v>-2.84339125983748E-2</v>
+        <v>-2.84339125983749E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12101,13 +12150,13 @@
         <v>0.5</v>
       </c>
       <c r="D35" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E35" s="8">
-        <v>0.12867122132689901</v>
+        <v>0.12893431014342599</v>
       </c>
       <c r="F35" s="8">
-        <v>-2.84339125983749E-2</v>
+        <v>-2.84339125983748E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12115,18 +12164,20 @@
         <v>5</v>
       </c>
       <c r="B36" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C36" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D36" s="9">
-        <v>0.01</v>
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0.2</v>
       </c>
       <c r="E36" s="8">
-        <v>-4.4793364376875297E-2</v>
-      </c>
-      <c r="F36" s="8"/>
+        <v>0.12867122132689901</v>
+      </c>
+      <c r="F36" s="8">
+        <v>-2.84339125983749E-2</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="7">
@@ -12139,12 +12190,14 @@
         <v>0.25</v>
       </c>
       <c r="D37" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E37" s="8">
         <v>-4.4793364376875297E-2</v>
       </c>
-      <c r="F37" s="8"/>
+      <c r="F37" s="8">
+        <v>8.7845794012064594E-3</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="7">
@@ -12156,14 +12209,14 @@
       <c r="C38" s="7">
         <v>0.25</v>
       </c>
-      <c r="D38" s="7">
-        <v>0.1</v>
+      <c r="D38" s="9">
+        <v>0.05</v>
       </c>
       <c r="E38" s="8">
-        <v>5.3416589194425601E-2</v>
+        <v>-4.4793364376875297E-2</v>
       </c>
       <c r="F38" s="8">
-        <v>8.7863724707500802E-3</v>
+        <v>8.7845794012064195E-3</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12177,13 +12230,13 @@
         <v>0.25</v>
       </c>
       <c r="D39" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E39" s="8">
-        <v>5.3416589194425802E-2</v>
+        <v>5.3416589194425601E-2</v>
       </c>
       <c r="F39" s="8">
-        <v>8.7845794012064299E-3</v>
+        <v>8.7863724707500802E-3</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12194,15 +12247,17 @@
         <v>5</v>
       </c>
       <c r="C40" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D40" s="9">
-        <v>0.01</v>
+        <v>0.25</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0.2</v>
       </c>
       <c r="E40" s="8">
-        <v>-0.11320154713019701</v>
-      </c>
-      <c r="F40" s="8"/>
+        <v>5.3416589194425802E-2</v>
+      </c>
+      <c r="F40" s="8">
+        <v>8.7845794012064299E-3</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="7">
@@ -12215,12 +12270,14 @@
         <v>0.5</v>
       </c>
       <c r="D41" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E41" s="8">
         <v>-0.11320154713019701</v>
       </c>
-      <c r="F41" s="8"/>
+      <c r="F41" s="8">
+        <v>1.06565678427087E-2</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A42" s="7">
@@ -12232,14 +12289,14 @@
       <c r="C42" s="7">
         <v>0.5</v>
       </c>
-      <c r="D42" s="7">
-        <v>0.1</v>
+      <c r="D42" s="9">
+        <v>0.05</v>
       </c>
       <c r="E42" s="8">
-        <v>-7.0282122882539599E-2</v>
+        <v>-0.11320154713019701</v>
       </c>
       <c r="F42" s="8">
-        <v>1.0656567842708801E-2</v>
+        <v>1.06565678427087E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12253,7 +12310,7 @@
         <v>0.5</v>
       </c>
       <c r="D43" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E43" s="8">
         <v>-7.0282122882539599E-2</v>
@@ -12267,18 +12324,20 @@
         <v>5</v>
       </c>
       <c r="B44" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C44" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D44" s="9">
-        <v>0.01</v>
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0.2</v>
       </c>
       <c r="E44" s="8">
-        <v>-8.4881321751472602E-2</v>
-      </c>
-      <c r="F44" s="8"/>
+        <v>-7.0282122882539599E-2</v>
+      </c>
+      <c r="F44" s="8">
+        <v>1.0656567842708801E-2</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A45" s="7">
@@ -12291,12 +12350,14 @@
         <v>0.25</v>
       </c>
       <c r="D45" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E45" s="8">
         <v>-8.4881321751472602E-2</v>
       </c>
-      <c r="F45" s="8"/>
+      <c r="F45" s="8">
+        <v>3.7713533408709802E-3</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A46" s="7">
@@ -12308,14 +12369,14 @@
       <c r="C46" s="7">
         <v>0.25</v>
       </c>
-      <c r="D46" s="7">
-        <v>0.1</v>
+      <c r="D46" s="9">
+        <v>0.05</v>
       </c>
       <c r="E46" s="8">
-        <v>2.2160466980396198E-2</v>
+        <v>-8.4881321751472602E-2</v>
       </c>
       <c r="F46" s="8">
-        <v>3.7713533408709702E-3</v>
+        <v>3.77135334087087E-3</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12329,13 +12390,13 @@
         <v>0.25</v>
       </c>
       <c r="D47" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E47" s="8">
-        <v>2.21598482080612E-2</v>
+        <v>2.2160466980396198E-2</v>
       </c>
       <c r="F47" s="8">
-        <v>3.7713533408709598E-3</v>
+        <v>3.7713533408709702E-3</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12346,15 +12407,17 @@
         <v>20</v>
       </c>
       <c r="C48" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D48" s="9">
-        <v>0.01</v>
+        <v>0.25</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0.2</v>
       </c>
       <c r="E48" s="8">
-        <v>-0.165584851919304</v>
-      </c>
-      <c r="F48" s="8"/>
+        <v>2.21598482080612E-2</v>
+      </c>
+      <c r="F48" s="8">
+        <v>3.7713533408709598E-3</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A49" s="7">
@@ -12367,12 +12430,14 @@
         <v>0.5</v>
       </c>
       <c r="D49" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E49" s="8">
         <v>-0.165584851919304</v>
       </c>
-      <c r="F49" s="8"/>
+      <c r="F49" s="8">
+        <v>8.8511386950288796E-3</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A50" s="7">
@@ -12384,14 +12449,14 @@
       <c r="C50" s="7">
         <v>0.5</v>
       </c>
-      <c r="D50" s="7">
-        <v>0.1</v>
+      <c r="D50" s="9">
+        <v>0.05</v>
       </c>
       <c r="E50" s="8">
-        <v>-0.12035305807387001</v>
+        <v>-0.165584851919304</v>
       </c>
       <c r="F50" s="8">
-        <v>8.8511386950287096E-3</v>
+        <v>8.8511386950287495E-3</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12405,39 +12470,41 @@
         <v>0.5</v>
       </c>
       <c r="D51" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E51" s="8">
+        <v>-0.12035305807387001</v>
+      </c>
+      <c r="F51" s="8">
+        <v>8.8511386950287096E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A52" s="7">
+        <v>5</v>
+      </c>
+      <c r="B52" s="7">
+        <v>20</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D52" s="7">
         <v>0.2</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E52" s="8">
         <v>-0.120353249554302</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F52" s="8">
         <v>8.8511386950288293E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-    </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A53" s="7">
-        <v>20</v>
-      </c>
-      <c r="B53" s="7">
-        <v>1</v>
-      </c>
-      <c r="C53" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D53" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="E53" s="8">
-        <v>0.14743629252229701</v>
-      </c>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="8"/>
     </row>
     <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12451,12 +12518,14 @@
         <v>0.25</v>
       </c>
       <c r="D54" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E54" s="8">
         <v>0.14743629252229701</v>
       </c>
-      <c r="F54" s="8"/>
+      <c r="F54" s="8">
+        <v>-5.88753318492405E-2</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A55" s="7">
@@ -12468,11 +12537,11 @@
       <c r="C55" s="7">
         <v>0.25</v>
       </c>
-      <c r="D55" s="7">
-        <v>0.1</v>
+      <c r="D55" s="9">
+        <v>0.05</v>
       </c>
       <c r="E55" s="8">
-        <v>0.15313922148498199</v>
+        <v>0.14743629252229701</v>
       </c>
       <c r="F55" s="8">
         <v>-5.88753318492405E-2</v>
@@ -12489,13 +12558,13 @@
         <v>0.25</v>
       </c>
       <c r="D56" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E56" s="8">
         <v>0.15313922148498199</v>
       </c>
       <c r="F56" s="8">
-        <v>-5.8875331849240597E-2</v>
+        <v>-5.88753318492405E-2</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12506,15 +12575,17 @@
         <v>1</v>
       </c>
       <c r="C57" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D57" s="9">
-        <v>0.01</v>
+        <v>0.25</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0.2</v>
       </c>
       <c r="E57" s="8">
-        <v>0.103763087815315</v>
-      </c>
-      <c r="F57" s="8"/>
+        <v>0.15313922148498199</v>
+      </c>
+      <c r="F57" s="8">
+        <v>-5.8875331849240597E-2</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A58" s="7">
@@ -12527,12 +12598,14 @@
         <v>0.5</v>
       </c>
       <c r="D58" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E58" s="8">
         <v>0.103763087815315</v>
       </c>
-      <c r="F58" s="8"/>
+      <c r="F58" s="8">
+        <v>-5.2610318220678097E-2</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A59" s="7">
@@ -12544,14 +12617,14 @@
       <c r="C59" s="7">
         <v>0.5</v>
       </c>
-      <c r="D59" s="7">
-        <v>0.1</v>
+      <c r="D59" s="9">
+        <v>0.05</v>
       </c>
       <c r="E59" s="8">
-        <v>0.13266509586470199</v>
+        <v>0.103763087815315</v>
       </c>
       <c r="F59" s="8">
-        <v>-5.2623625398156099E-2</v>
+        <v>-5.2610318220678097E-2</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12565,7 +12638,7 @@
         <v>0.5</v>
       </c>
       <c r="D60" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E60" s="8">
         <v>0.13266509586470199</v>
@@ -12579,18 +12652,20 @@
         <v>20</v>
       </c>
       <c r="B61" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C61" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D61" s="9">
-        <v>0.01</v>
+        <v>0.5</v>
+      </c>
+      <c r="D61" s="7">
+        <v>0.2</v>
       </c>
       <c r="E61" s="8">
-        <v>9.8642849217424694E-2</v>
-      </c>
-      <c r="F61" s="8"/>
+        <v>0.13266509586470199</v>
+      </c>
+      <c r="F61" s="8">
+        <v>-5.2623625398156099E-2</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A62" s="7">
@@ -12603,12 +12678,14 @@
         <v>0.25</v>
       </c>
       <c r="D62" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E62" s="8">
-        <v>9.8642849217424597E-2</v>
-      </c>
-      <c r="F62" s="8"/>
+        <v>9.8642849217424694E-2</v>
+      </c>
+      <c r="F62" s="8">
+        <v>-3.6518484126942898E-2</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A63" s="7">
@@ -12620,11 +12697,11 @@
       <c r="C63" s="7">
         <v>0.25</v>
       </c>
-      <c r="D63" s="7">
-        <v>0.1</v>
+      <c r="D63" s="9">
+        <v>0.05</v>
       </c>
       <c r="E63" s="8">
-        <v>0.108027884460389</v>
+        <v>9.8642849217424597E-2</v>
       </c>
       <c r="F63" s="8">
         <v>-3.6518484126942898E-2</v>
@@ -12641,7 +12718,7 @@
         <v>0.25</v>
       </c>
       <c r="D64" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E64" s="8">
         <v>0.108027884460389</v>
@@ -12658,15 +12735,17 @@
         <v>5</v>
       </c>
       <c r="C65" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D65" s="9">
-        <v>0.01</v>
+        <v>0.25</v>
+      </c>
+      <c r="D65" s="7">
+        <v>0.2</v>
       </c>
       <c r="E65" s="8">
-        <v>-1.8755832844895199E-2</v>
-      </c>
-      <c r="F65" s="8"/>
+        <v>0.108027884460389</v>
+      </c>
+      <c r="F65" s="8">
+        <v>-3.6518484126942898E-2</v>
+      </c>
     </row>
     <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A66" s="7">
@@ -12679,12 +12758,14 @@
         <v>0.5</v>
       </c>
       <c r="D66" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E66" s="8">
         <v>-1.8755832844895199E-2</v>
       </c>
-      <c r="F66" s="8"/>
+      <c r="F66" s="8">
+        <v>-2.6042330806943698E-2</v>
+      </c>
     </row>
     <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A67" s="7">
@@ -12696,14 +12777,14 @@
       <c r="C67" s="7">
         <v>0.5</v>
       </c>
-      <c r="D67" s="7">
-        <v>0.1</v>
+      <c r="D67" s="9">
+        <v>0.05</v>
       </c>
       <c r="E67" s="8">
-        <v>2.3965435250042199E-2</v>
+        <v>-1.8755832844895199E-2</v>
       </c>
       <c r="F67" s="8">
-        <v>-2.6042330806943799E-2</v>
+        <v>-2.6042330806943698E-2</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12717,13 +12798,13 @@
         <v>0.5</v>
       </c>
       <c r="D68" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E68" s="8">
         <v>2.3965435250042199E-2</v>
       </c>
       <c r="F68" s="8">
-        <v>-2.6063045074091799E-2</v>
+        <v>-2.6042330806943799E-2</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12731,18 +12812,20 @@
         <v>20</v>
       </c>
       <c r="B69" s="7">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C69" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D69" s="9">
-        <v>0.01</v>
+        <v>0.5</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0.2</v>
       </c>
       <c r="E69" s="8">
-        <v>8.1108723348584599E-2</v>
-      </c>
-      <c r="F69" s="8"/>
+        <v>2.3965435250042199E-2</v>
+      </c>
+      <c r="F69" s="8">
+        <v>-2.6063045074091799E-2</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A70" s="7">
@@ -12755,12 +12838,14 @@
         <v>0.25</v>
       </c>
       <c r="D70" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E70" s="8">
-        <v>8.1108723348584794E-2</v>
-      </c>
-      <c r="F70" s="8"/>
+        <v>8.1108723348584599E-2</v>
+      </c>
+      <c r="F70" s="8">
+        <v>-4.2581416135986698E-2</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A71" s="7">
@@ -12772,14 +12857,14 @@
       <c r="C71" s="7">
         <v>0.25</v>
       </c>
-      <c r="D71" s="7">
-        <v>0.1</v>
+      <c r="D71" s="9">
+        <v>0.05</v>
       </c>
       <c r="E71" s="8">
-        <v>9.1612494841683406E-2</v>
+        <v>8.1108723348584794E-2</v>
       </c>
       <c r="F71" s="8">
-        <v>-4.2581416135986698E-2</v>
+        <v>-4.2581416135986802E-2</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12793,13 +12878,13 @@
         <v>0.25</v>
       </c>
       <c r="D72" s="7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E72" s="8">
-        <v>9.1614115691380504E-2</v>
+        <v>9.1612494841683406E-2</v>
       </c>
       <c r="F72" s="8">
-        <v>-4.2581416135986802E-2</v>
+        <v>-4.2581416135986698E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12810,15 +12895,17 @@
         <v>20</v>
       </c>
       <c r="C73" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D73" s="9">
-        <v>0.01</v>
+        <v>0.25</v>
+      </c>
+      <c r="D73" s="7">
+        <v>0.2</v>
       </c>
       <c r="E73" s="8">
-        <v>-5.5297737433492901E-2</v>
-      </c>
-      <c r="F73" s="8"/>
+        <v>9.1614115691380504E-2</v>
+      </c>
+      <c r="F73" s="8">
+        <v>-4.2581416135986802E-2</v>
+      </c>
     </row>
     <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A74" s="7">
@@ -12831,12 +12918,14 @@
         <v>0.5</v>
       </c>
       <c r="D74" s="9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E74" s="8">
-        <v>-5.5297737433492797E-2</v>
-      </c>
-      <c r="F74" s="8"/>
+        <v>-5.5297737433492901E-2</v>
+      </c>
+      <c r="F74" s="8">
+        <v>-4.13107001371062E-2</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A75" s="7">
@@ -12848,14 +12937,14 @@
       <c r="C75" s="7">
         <v>0.5</v>
       </c>
-      <c r="D75" s="7">
-        <v>0.1</v>
+      <c r="D75" s="9">
+        <v>0.05</v>
       </c>
       <c r="E75" s="8">
-        <v>-9.2409072476452997E-3</v>
+        <v>-5.5297737433492797E-2</v>
       </c>
       <c r="F75" s="8">
-        <v>-4.13107001371062E-2</v>
+        <v>-4.1310700137106297E-2</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.15">
@@ -12869,12 +12958,32 @@
         <v>0.5</v>
       </c>
       <c r="D76" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E76" s="8">
+        <v>-9.2409072476452997E-3</v>
+      </c>
+      <c r="F76" s="8">
+        <v>-4.13107001371062E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A77" s="7">
+        <v>20</v>
+      </c>
+      <c r="B77" s="7">
+        <v>20</v>
+      </c>
+      <c r="C77" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D77" s="7">
         <v>0.2</v>
       </c>
-      <c r="E76" s="8">
+      <c r="E77" s="8">
         <v>-9.2410588069189708E-3</v>
       </c>
-      <c r="F76" s="8">
+      <c r="F77" s="8">
         <v>-4.1321897718647402E-2</v>
       </c>
     </row>

</xml_diff>